<commit_message>
VL Variation fertig, kNW V0 etspricht bisher original (sollte so sein)
</commit_message>
<xml_diff>
--- a/9_2_VLT_Variation/9_2_FBH_Einfluss_VLT.xlsx
+++ b/9_2_VLT_Variation/9_2_FBH_Einfluss_VLT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fraunhofer-my.sharepoint.com/personal/lara_josephine_barnic_iee_fraunhofer_de/Documents/A_Bearbeitung/9_Parameterstudie_REP/9_2_VLT_Variation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{E194A4E9-0780-4D2C-85A2-5935A5786084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2424C3B-76E5-466B-971A-47882BBD4186}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="8_{E194A4E9-0780-4D2C-85A2-5935A5786084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FA16A89-9171-4927-A296-70C3F2A22DBA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{0F735A68-00BF-458F-A0D9-4A275F93B0FE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{0F735A68-00BF-458F-A0D9-4A275F93B0FE}"/>
   </bookViews>
   <sheets>
     <sheet name="VLT_jeHaus_FBH" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="67">
   <si>
     <t>Beispielrechnung</t>
   </si>
@@ -265,6 +265,9 @@
   </si>
   <si>
     <t>Ambitioniert</t>
+  </si>
+  <si>
+    <t>Heizkörperexponent Einfluss --&gt; VLT, RLT</t>
   </si>
 </sst>
 </file>
@@ -273,7 +276,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -418,14 +421,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -434,13 +440,10 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -470,13 +473,13 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>752476</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>47626</xdr:rowOff>
+      <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>79668</xdr:rowOff>
+      <xdr:rowOff>108243</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -499,7 +502,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7610476" y="47626"/>
+          <a:off x="7610476" y="76201"/>
           <a:ext cx="3905249" cy="1956092"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -517,8 +520,8 @@
       <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2401042" cy="535275"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="Textfeld 2">
@@ -851,7 +854,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="Textfeld 2">
@@ -1030,6 +1033,439 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2401042" cy="535275"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="Textfeld 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29A68BED-6DC4-47AE-807F-6D37ECDFAAD5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11430000" y="3648075"/>
+              <a:ext cx="2401042" cy="535275"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1400" i="1" kern="1200">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>∆</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1400" b="0" i="1" kern="1200">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1400" i="1" kern="1200">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝜗</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1400" b="0" i="1" kern="1200">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑛𝑒𝑢</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1400" b="0" i="1" kern="1200">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1400" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>∆</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1400" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝜗</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑁𝑜𝑟𝑚</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>∗</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:f>
+                              <m:fPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                                    <a:solidFill>
+                                      <a:schemeClr val="tx1"/>
+                                    </a:solidFill>
+                                    <a:effectLst/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="+mn-ea"/>
+                                    <a:cs typeface="+mn-cs"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:fPr>
+                              <m:num>
+                                <m:sSub>
+                                  <m:sSubPr>
+                                    <m:ctrlPr>
+                                      <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                                        <a:solidFill>
+                                          <a:schemeClr val="tx1"/>
+                                        </a:solidFill>
+                                        <a:effectLst/>
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                        <a:ea typeface="+mn-ea"/>
+                                        <a:cs typeface="+mn-cs"/>
+                                      </a:rPr>
+                                    </m:ctrlPr>
+                                  </m:sSubPr>
+                                  <m:e>
+                                    <m:r>
+                                      <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                                        <a:solidFill>
+                                          <a:schemeClr val="tx1"/>
+                                        </a:solidFill>
+                                        <a:effectLst/>
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                        <a:ea typeface="+mn-ea"/>
+                                        <a:cs typeface="+mn-cs"/>
+                                      </a:rPr>
+                                      <m:t>𝑄</m:t>
+                                    </m:r>
+                                  </m:e>
+                                  <m:sub>
+                                    <m:r>
+                                      <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                                        <a:solidFill>
+                                          <a:schemeClr val="tx1"/>
+                                        </a:solidFill>
+                                        <a:effectLst/>
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                        <a:ea typeface="+mn-ea"/>
+                                        <a:cs typeface="+mn-cs"/>
+                                      </a:rPr>
+                                      <m:t>𝑛𝑒𝑢</m:t>
+                                    </m:r>
+                                  </m:sub>
+                                </m:sSub>
+                              </m:num>
+                              <m:den>
+                                <m:sSub>
+                                  <m:sSubPr>
+                                    <m:ctrlPr>
+                                      <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                                        <a:solidFill>
+                                          <a:schemeClr val="tx1"/>
+                                        </a:solidFill>
+                                        <a:effectLst/>
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                        <a:ea typeface="+mn-ea"/>
+                                        <a:cs typeface="+mn-cs"/>
+                                      </a:rPr>
+                                    </m:ctrlPr>
+                                  </m:sSubPr>
+                                  <m:e>
+                                    <m:r>
+                                      <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                                        <a:solidFill>
+                                          <a:schemeClr val="tx1"/>
+                                        </a:solidFill>
+                                        <a:effectLst/>
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                        <a:ea typeface="+mn-ea"/>
+                                        <a:cs typeface="+mn-cs"/>
+                                      </a:rPr>
+                                      <m:t>𝑄</m:t>
+                                    </m:r>
+                                  </m:e>
+                                  <m:sub>
+                                    <m:r>
+                                      <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                                        <a:solidFill>
+                                          <a:schemeClr val="tx1"/>
+                                        </a:solidFill>
+                                        <a:effectLst/>
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                        <a:ea typeface="+mn-ea"/>
+                                        <a:cs typeface="+mn-cs"/>
+                                      </a:rPr>
+                                      <m:t>𝑁𝑜𝑟𝑚</m:t>
+                                    </m:r>
+                                  </m:sub>
+                                </m:sSub>
+                              </m:den>
+                            </m:f>
+                          </m:e>
+                        </m:d>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>1/</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑛</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="de-DE" sz="1400" kern="1200"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="Textfeld 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29A68BED-6DC4-47AE-807F-6D37ECDFAAD5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11430000" y="3648075"/>
+              <a:ext cx="2401042" cy="535275"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1400" i="0" kern="1200">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>∆𝜗</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1400" b="0" i="0" kern="1200">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_𝑛𝑒𝑢=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1400" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>∆𝜗</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1400" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_𝑁𝑜𝑟𝑚∗(𝑄_𝑛𝑒𝑢/𝑄_𝑁𝑜𝑟𝑚 )^(1/𝑛)</a:t>
+              </a:r>
+              <a:endParaRPr lang="de-DE" sz="1400" kern="1200"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1064,9 +1500,6 @@
           </cell>
         </row>
         <row r="3">
-          <cell r="C3">
-            <v>141.9112910905414</v>
-          </cell>
           <cell r="D3">
             <v>127.3212049729668</v>
           </cell>
@@ -1075,9 +1508,6 @@
           </cell>
         </row>
         <row r="4">
-          <cell r="C4">
-            <v>133.33954555201521</v>
-          </cell>
           <cell r="D4">
             <v>112.867449169975</v>
           </cell>
@@ -1086,9 +1516,6 @@
           </cell>
         </row>
         <row r="5">
-          <cell r="C5">
-            <v>35.58219185276743</v>
-          </cell>
           <cell r="D5">
             <v>32.747186449920051</v>
           </cell>
@@ -1467,8 +1894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B1631A3-5489-4862-B1F9-D2CC6DD97E5C}">
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="M48" sqref="M48"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="S43" sqref="S43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,12 +1942,12 @@
       <c r="I3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="Q3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F4" s="2" t="s">
@@ -1535,10 +1962,10 @@
       <c r="I4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F5" s="2" t="s">
@@ -1550,10 +1977,10 @@
       <c r="I5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F6" s="2" t="s">
@@ -1565,10 +1992,10 @@
       <c r="I6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
     </row>
     <row r="7" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -1583,10 +2010,10 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F8" s="2" t="s">
@@ -1601,10 +2028,10 @@
       <c r="I8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F9" s="2" t="s">
@@ -1619,10 +2046,10 @@
       <c r="I9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F10" s="2" t="s">
@@ -1637,10 +2064,10 @@
       <c r="I10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F11" s="2" t="s">
@@ -1649,23 +2076,23 @@
       <c r="G11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="8">
         <f>(H9-H10)/ LN((H9-H3)/(H10-H3))</f>
         <v>48.829457165342603</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="I11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
     </row>
     <row r="13" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1680,10 +2107,10 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F14" s="2" t="s">
@@ -1698,16 +2125,16 @@
       <c r="I14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F16" s="2" t="s">
@@ -1716,33 +2143,33 @@
       <c r="G16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="8">
         <f>H11*(H14/H8)^(1/H4)</f>
         <v>36.622092874006952</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="I16" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="8">
         <f>H11-H16</f>
         <v>12.207364291335651</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="I18" s="9" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1767,7 +2194,7 @@
       <c r="G21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="8">
         <f>H9-H18</f>
         <v>62.792635708664349</v>
       </c>
@@ -1782,7 +2209,7 @@
       <c r="G22" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="8">
         <f>H10-H18</f>
         <v>52.792635708664349</v>
       </c>
@@ -1833,34 +2260,39 @@
       <c r="G27" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H27" s="8">
         <f>(H24-H25) / LN((H24-H3)/(H25-H3))</f>
         <v>39.28812045180161</v>
       </c>
-      <c r="I27" s="10" t="s">
+      <c r="I27" s="9" t="s">
         <v>23</v>
       </c>
     </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R29" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="H31" s="11" t="s">
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="H31" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="M31" s="11" t="s">
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="M31" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="N31" s="11"/>
-      <c r="O31" s="11"/>
-      <c r="P31" s="11"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
     </row>
     <row r="32" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
@@ -1998,109 +2430,104 @@
       <c r="F35"/>
     </row>
     <row r="36" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="H36" s="13" t="s">
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="H36" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C37" s="6">
-        <f>ROUND('[1]max Wärmebedarfe_import'!C2,0)</f>
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D37" s="6">
-        <f>ROUND('[1]max Wärmebedarfe_import'!C3,0)</f>
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="E37" s="6">
-        <f>ROUND('[1]max Wärmebedarfe_import'!C4,0)</f>
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="F37" s="6">
-        <f>ROUND('[1]max Wärmebedarfe_import'!C5,0)</f>
-        <v>36</v>
-      </c>
-      <c r="H37" s="6" cm="1">
-        <f t="array" ref="H37:K37">C37:F37</f>
-        <v>51</v>
+        <v>33</v>
+      </c>
+      <c r="H37" s="6">
+        <v>32</v>
       </c>
       <c r="I37" s="6">
-        <v>142</v>
+        <v>98</v>
       </c>
       <c r="J37" s="6">
-        <v>133</v>
+        <v>94</v>
       </c>
       <c r="K37" s="6">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="M37" s="6" cm="1">
         <f t="array" ref="M37:P40">H37:K40</f>
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="N37" s="6">
-        <v>142</v>
+        <v>98</v>
       </c>
       <c r="O37" s="6">
-        <v>133</v>
+        <v>94</v>
       </c>
       <c r="P37" s="6">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C38" s="6">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="D38" s="6">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="E38" s="6">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="F38" s="6">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="H38" s="6">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="I38" s="6">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="J38" s="6">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="K38" s="6">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="M38" s="6">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="N38" s="6">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="O38" s="6">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="P38" s="6">
-        <v>75</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -2108,90 +2535,90 @@
         <v>20</v>
       </c>
       <c r="C39" s="6">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="D39" s="6">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="E39" s="6">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="F39" s="6">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="H39" s="6">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="I39" s="6">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="J39" s="6">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="K39" s="6">
-        <v>65</v>
-      </c>
-      <c r="L39" s="15"/>
+        <v>30</v>
+      </c>
+      <c r="L39" s="11"/>
       <c r="M39" s="6">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="N39" s="6">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="O39" s="6">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="P39" s="6">
-        <v>65</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C40" s="9">
+      <c r="C40" s="8">
         <f>(C38-C39)/ LN((C38-C33)/(C39-C33))</f>
-        <v>48.829457165342603</v>
-      </c>
-      <c r="D40" s="9">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="D40" s="8">
         <f>(D38-D39)/ LN((D38-D33)/(D39-D33))</f>
-        <v>48.829457165342603</v>
-      </c>
-      <c r="E40" s="9">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="E40" s="8">
         <f>(E38-E39)/ LN((E38-E33)/(E39-E33))</f>
-        <v>48.829457165342603</v>
-      </c>
-      <c r="F40" s="9">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="F40" s="8">
         <f>(F38-F39)/ LN((F38-F33)/(F39-F33))</f>
-        <v>48.829457165342603</v>
-      </c>
-      <c r="H40" s="9">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="H40" s="8">
         <f>(H38-H39)/ LN((H38-H33)/(H39-H33))</f>
-        <v>48.829457165342603</v>
-      </c>
-      <c r="I40" s="9">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="I40" s="8">
         <f>(I38-I39)/ LN((I38-I33)/(I39-I33))</f>
-        <v>48.829457165342603</v>
-      </c>
-      <c r="J40" s="9">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="J40" s="8">
         <f>(J38-J39)/ LN((J38-J33)/(J39-J33))</f>
-        <v>48.829457165342603</v>
-      </c>
-      <c r="K40" s="9">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="K40" s="8">
         <f>(K38-K39)/ LN((K38-K33)/(K39-K33))</f>
-        <v>48.829457165342603</v>
-      </c>
-      <c r="M40" s="9">
-        <v>48.829457165342603</v>
-      </c>
-      <c r="N40" s="9">
-        <v>48.829457165342603</v>
-      </c>
-      <c r="O40" s="9">
-        <v>48.829457165342603</v>
-      </c>
-      <c r="P40" s="9">
-        <v>48.829457165342603</v>
+        <v>11.316499227839616</v>
+      </c>
+      <c r="M40" s="8">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="N40" s="8">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="O40" s="8">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="P40" s="8">
+        <v>11.316499227839616</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -2199,19 +2626,19 @@
       <c r="F41"/>
     </row>
     <row r="42" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="H42" s="13" t="s">
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="H42" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I42" s="13"/>
-      <c r="J42" s="13"/>
-      <c r="K42" s="13"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
@@ -2258,37 +2685,37 @@
       <c r="B45" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C45" s="9">
+      <c r="C45" s="8">
         <f>C40*(C43/C37)^(1/C34)</f>
-        <v>42.127374809315192</v>
-      </c>
-      <c r="D45" s="9">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="D45" s="8">
         <f>D40*(D43/D37)^(1/D34)</f>
-        <v>43.67141591548247</v>
-      </c>
-      <c r="E45" s="9">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="E45" s="8">
         <f>E40*(E43/E37)^(1/E34)</f>
-        <v>41.486681651757252</v>
-      </c>
-      <c r="F45" s="9">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="F45" s="8">
         <f>F40*(F43/F37)^(1/F34)</f>
-        <v>44.760335734897382</v>
-      </c>
-      <c r="H45" s="9">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="H45" s="8">
         <f>H40*(H43/H37)^(1/H34)</f>
-        <v>30.638090770411043</v>
-      </c>
-      <c r="I45" s="9">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="I45" s="8">
         <f>I40*(I43/I37)^(1/I34)</f>
-        <v>33.699202832419545</v>
-      </c>
-      <c r="J45" s="9">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="J45" s="8">
         <f>J40*(J43/J37)^(1/J34)</f>
-        <v>34.511044913851158</v>
-      </c>
-      <c r="K45" s="9">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="K45" s="8">
         <f>K40*(K43/K37)^(1/K34)</f>
-        <v>27.127476202968115</v>
+        <v>11.316499227839616</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -2299,37 +2726,37 @@
       <c r="B47" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="9">
+      <c r="C47" s="8">
         <f>C40-C45</f>
-        <v>6.702082356027411</v>
-      </c>
-      <c r="D47" s="9">
+        <v>0</v>
+      </c>
+      <c r="D47" s="8">
         <f>D40-D45</f>
-        <v>5.1580412498601333</v>
-      </c>
-      <c r="E47" s="9">
+        <v>0</v>
+      </c>
+      <c r="E47" s="8">
         <f>E40-E45</f>
-        <v>7.3427755135853516</v>
-      </c>
-      <c r="F47" s="9">
+        <v>0</v>
+      </c>
+      <c r="F47" s="8">
         <f>F40-F45</f>
-        <v>4.0691214304452217</v>
-      </c>
-      <c r="H47" s="9">
+        <v>0</v>
+      </c>
+      <c r="H47" s="8">
         <f>H40-H45</f>
-        <v>18.19136639493156</v>
-      </c>
-      <c r="I47" s="9">
+        <v>0</v>
+      </c>
+      <c r="I47" s="8">
         <f>I40-I45</f>
-        <v>15.130254332923059</v>
-      </c>
-      <c r="J47" s="9">
+        <v>0</v>
+      </c>
+      <c r="J47" s="8">
         <f>J40-J45</f>
-        <v>14.318412251491445</v>
-      </c>
-      <c r="K47" s="9">
+        <v>0</v>
+      </c>
+      <c r="K47" s="8">
         <f>K40-K45</f>
-        <v>21.701980962374488</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -2337,92 +2764,92 @@
       <c r="F48"/>
     </row>
     <row r="49" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
-      <c r="H49" s="13" t="s">
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="H49" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="I49" s="13"/>
-      <c r="J49" s="13"/>
-      <c r="K49" s="13"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="14"/>
+      <c r="K49" s="14"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C50" s="9">
+      <c r="C50" s="8">
         <f>C38-C47</f>
-        <v>68.297917643972596</v>
-      </c>
-      <c r="D50" s="9">
+        <v>35</v>
+      </c>
+      <c r="D50" s="8">
         <f>D38-D47</f>
-        <v>69.841958750139867</v>
-      </c>
-      <c r="E50" s="9">
+        <v>35</v>
+      </c>
+      <c r="E50" s="8">
         <f>E38-E47</f>
-        <v>67.657224486414648</v>
-      </c>
-      <c r="F50" s="9">
+        <v>35</v>
+      </c>
+      <c r="F50" s="8">
         <f>F38-F47</f>
-        <v>70.930878569554778</v>
-      </c>
-      <c r="H50" s="9">
+        <v>35</v>
+      </c>
+      <c r="H50" s="8">
         <f>H38-H47</f>
-        <v>56.808633605068437</v>
-      </c>
-      <c r="I50" s="9">
+        <v>35</v>
+      </c>
+      <c r="I50" s="8">
         <f>I38-I47</f>
-        <v>59.869745667076941</v>
-      </c>
-      <c r="J50" s="9">
+        <v>35</v>
+      </c>
+      <c r="J50" s="8">
         <f>J38-J47</f>
-        <v>60.681587748508555</v>
-      </c>
-      <c r="K50" s="9">
+        <v>35</v>
+      </c>
+      <c r="K50" s="8">
         <f>K38-K47</f>
-        <v>53.298019037625508</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C51" s="9">
+      <c r="C51" s="8">
         <f>C39-C47</f>
-        <v>58.297917643972589</v>
-      </c>
-      <c r="D51" s="9">
+        <v>30</v>
+      </c>
+      <c r="D51" s="8">
         <f>D39-D47</f>
-        <v>59.841958750139867</v>
-      </c>
-      <c r="E51" s="9">
+        <v>30</v>
+      </c>
+      <c r="E51" s="8">
         <f>E39-E47</f>
-        <v>57.657224486414648</v>
-      </c>
-      <c r="F51" s="9">
+        <v>30</v>
+      </c>
+      <c r="F51" s="8">
         <f>F39-F47</f>
-        <v>60.930878569554778</v>
-      </c>
-      <c r="H51" s="9">
+        <v>30</v>
+      </c>
+      <c r="H51" s="8">
         <f>H39-H47</f>
-        <v>46.808633605068437</v>
-      </c>
-      <c r="I51" s="9">
+        <v>30</v>
+      </c>
+      <c r="I51" s="8">
         <f>I39-I47</f>
-        <v>49.869745667076941</v>
-      </c>
-      <c r="J51" s="9">
+        <v>30</v>
+      </c>
+      <c r="J51" s="8">
         <f>J39-J47</f>
-        <v>50.681587748508555</v>
-      </c>
-      <c r="K51" s="9">
+        <v>30</v>
+      </c>
+      <c r="K51" s="8">
         <f>K39-K47</f>
-        <v>43.298019037625508</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
@@ -2432,74 +2859,74 @@
       <c r="B53" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C53" s="16">
+      <c r="C53" s="12">
         <f>ROUND(C50,1)</f>
-        <v>68.3</v>
-      </c>
-      <c r="D53" s="16">
+        <v>35</v>
+      </c>
+      <c r="D53" s="12">
         <f t="shared" ref="D53:F53" si="1">ROUND(D50,1)</f>
-        <v>69.8</v>
-      </c>
-      <c r="E53" s="16">
+        <v>35</v>
+      </c>
+      <c r="E53" s="12">
         <f t="shared" si="1"/>
-        <v>67.7</v>
-      </c>
-      <c r="F53" s="16">
+        <v>35</v>
+      </c>
+      <c r="F53" s="12">
         <f t="shared" si="1"/>
-        <v>70.900000000000006</v>
-      </c>
-      <c r="H53" s="16">
+        <v>35</v>
+      </c>
+      <c r="H53" s="12">
         <f>ROUND(H50,1)</f>
-        <v>56.8</v>
-      </c>
-      <c r="I53" s="16">
+        <v>35</v>
+      </c>
+      <c r="I53" s="12">
         <f t="shared" ref="I53:K54" si="2">ROUND(I50,1)</f>
-        <v>59.9</v>
-      </c>
-      <c r="J53" s="16">
+        <v>35</v>
+      </c>
+      <c r="J53" s="12">
         <f t="shared" si="2"/>
-        <v>60.7</v>
-      </c>
-      <c r="K53" s="16">
+        <v>35</v>
+      </c>
+      <c r="K53" s="12">
         <f t="shared" si="2"/>
-        <v>53.3</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C54" s="16">
+      <c r="C54" s="12">
         <f>ROUND(C51,1)</f>
-        <v>58.3</v>
-      </c>
-      <c r="D54" s="16">
+        <v>30</v>
+      </c>
+      <c r="D54" s="12">
         <f t="shared" ref="D54:F54" si="3">ROUND(D51,1)</f>
-        <v>59.8</v>
-      </c>
-      <c r="E54" s="16">
+        <v>30</v>
+      </c>
+      <c r="E54" s="12">
         <f t="shared" si="3"/>
-        <v>57.7</v>
-      </c>
-      <c r="F54" s="16">
+        <v>30</v>
+      </c>
+      <c r="F54" s="12">
         <f t="shared" si="3"/>
-        <v>60.9</v>
-      </c>
-      <c r="H54" s="16">
+        <v>30</v>
+      </c>
+      <c r="H54" s="12">
         <f>ROUND(H51,1)</f>
-        <v>46.8</v>
-      </c>
-      <c r="I54" s="16">
+        <v>30</v>
+      </c>
+      <c r="I54" s="12">
         <f t="shared" si="2"/>
-        <v>49.9</v>
-      </c>
-      <c r="J54" s="16">
+        <v>30</v>
+      </c>
+      <c r="J54" s="12">
         <f t="shared" si="2"/>
-        <v>50.7</v>
-      </c>
-      <c r="K54" s="16">
+        <v>30</v>
+      </c>
+      <c r="K54" s="12">
         <f t="shared" si="2"/>
-        <v>43.3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
@@ -2509,37 +2936,37 @@
       <c r="B56" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C56" s="9">
+      <c r="C56" s="8">
         <f>(C53-C54) / LN((C53-C33)/(C54-C33))</f>
-        <v>42.102255045173635</v>
-      </c>
-      <c r="D56" s="9">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="D56" s="8">
         <f>(D53-D54) / LN((D53-D33)/(D54-D33))</f>
-        <v>43.60907553868752</v>
-      </c>
-      <c r="E56" s="9">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="E56" s="8">
         <f>(E53-E54) / LN((E53-E33)/(E54-E33))</f>
-        <v>41.499387888201113</v>
-      </c>
-      <c r="F56" s="9">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="F56" s="8">
         <f>(F53-F54) / LN((F53-F33)/(F54-F33))</f>
-        <v>44.713784610927043</v>
-      </c>
-      <c r="H56" s="9">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="H56" s="8">
         <f>(H53-H54) / LN((H53-H33)/(H54-H33))</f>
-        <v>30.527509116574436</v>
-      </c>
-      <c r="I56" s="9">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="I56" s="8">
         <f>(I53-I54) / LN((I53-I33)/(I54-I33))</f>
-        <v>33.652736446091119</v>
-      </c>
-      <c r="J56" s="9">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="J56" s="8">
         <f>(J53-J54) / LN((J53-J33)/(J54-J33))</f>
-        <v>34.458501987818885</v>
-      </c>
-      <c r="K56" s="9">
+        <v>11.316499227839616</v>
+      </c>
+      <c r="K56" s="8">
         <f>(K53-K54) / LN((K53-K33)/(K54-K33))</f>
-        <v>26.991970165304586</v>
+        <v>11.316499227839616</v>
       </c>
     </row>
   </sheetData>
@@ -2565,8 +2992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05B082C0-AFA6-4F53-9FDC-E380FD125F52}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2625,12 +3052,10 @@
         <v>41</v>
       </c>
       <c r="B3">
-        <f>VLT_jeHaus_FBH!H53</f>
-        <v>56.8</v>
+        <v>35</v>
       </c>
       <c r="C3">
-        <f>VLT_jeHaus_FBH!H54</f>
-        <v>46.8</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <f>[2]VLT_jeHaus!H6</f>
@@ -2645,7 +3070,7 @@
       </c>
       <c r="G3">
         <f>VLT_jeHaus_FBH!H56</f>
-        <v>30.527509116574436</v>
+        <v>11.316499227839616</v>
       </c>
       <c r="H3">
         <f>VLT_jeHaus_FBH!H5</f>
@@ -2657,12 +3082,10 @@
         <v>42</v>
       </c>
       <c r="B4">
-        <f>VLT_jeHaus_FBH!I53</f>
-        <v>59.9</v>
+        <v>35</v>
       </c>
       <c r="C4">
-        <f>VLT_jeHaus_FBH!I54</f>
-        <v>49.9</v>
+        <v>30</v>
       </c>
       <c r="D4" cm="1">
         <f t="array" ref="D4:F4">D3:F3</f>
@@ -2676,7 +3099,7 @@
       </c>
       <c r="G4">
         <f>VLT_jeHaus_FBH!I56</f>
-        <v>33.652736446091119</v>
+        <v>11.316499227839616</v>
       </c>
       <c r="H4">
         <f>H3</f>
@@ -2688,12 +3111,10 @@
         <v>43</v>
       </c>
       <c r="B5">
-        <f>VLT_jeHaus_FBH!J53</f>
-        <v>60.7</v>
+        <v>35</v>
       </c>
       <c r="C5">
-        <f>VLT_jeHaus_FBH!J54</f>
-        <v>50.7</v>
+        <v>30</v>
       </c>
       <c r="D5" cm="1">
         <f t="array" ref="D5:F5">D3:F3</f>
@@ -2707,7 +3128,7 @@
       </c>
       <c r="G5">
         <f>VLT_jeHaus_FBH!J56</f>
-        <v>34.458501987818885</v>
+        <v>11.316499227839616</v>
       </c>
       <c r="H5">
         <f t="shared" ref="H5:H6" si="0">H4</f>
@@ -2719,12 +3140,10 @@
         <v>44</v>
       </c>
       <c r="B6">
-        <f>VLT_jeHaus_FBH!K53</f>
-        <v>53.3</v>
+        <v>35</v>
       </c>
       <c r="C6">
-        <f>VLT_jeHaus_FBH!K54</f>
-        <v>43.3</v>
+        <v>30</v>
       </c>
       <c r="D6" cm="1">
         <f t="array" ref="D6:F6">D3:F3</f>
@@ -2738,7 +3157,7 @@
       </c>
       <c r="G6">
         <f>VLT_jeHaus_FBH!K56</f>
-        <v>26.991970165304586</v>
+        <v>11.316499227839616</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
@@ -2754,8 +3173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD6CFE54-094C-46EC-AE96-7FD92F7B6210}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2818,11 +3237,11 @@
       </c>
       <c r="B3">
         <f>VLT_jeHaus_FBH!C53</f>
-        <v>68.3</v>
+        <v>35</v>
       </c>
       <c r="C3">
         <f>VLT_jeHaus_FBH!C54</f>
-        <v>58.3</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <f>[2]VLT_jeHaus!H6</f>
@@ -2837,7 +3256,7 @@
       </c>
       <c r="G3">
         <f>VLT_jeHaus_FBH!C56</f>
-        <v>42.102255045173635</v>
+        <v>11.316499227839616</v>
       </c>
       <c r="H3">
         <f>[2]VLT_jeHaus!H5</f>
@@ -2850,11 +3269,11 @@
       </c>
       <c r="B4">
         <f>VLT_jeHaus_FBH!D53</f>
-        <v>69.8</v>
+        <v>35</v>
       </c>
       <c r="C4">
         <f>VLT_jeHaus_FBH!D54</f>
-        <v>59.8</v>
+        <v>30</v>
       </c>
       <c r="D4" cm="1">
         <f t="array" ref="D4:F4">D3:F3</f>
@@ -2868,7 +3287,7 @@
       </c>
       <c r="G4">
         <f>VLT_jeHaus_FBH!D56</f>
-        <v>43.60907553868752</v>
+        <v>11.316499227839616</v>
       </c>
       <c r="H4">
         <f>H3</f>
@@ -2881,11 +3300,11 @@
       </c>
       <c r="B5">
         <f>VLT_jeHaus_FBH!E53</f>
-        <v>67.7</v>
+        <v>35</v>
       </c>
       <c r="C5">
         <f>VLT_jeHaus_FBH!E54</f>
-        <v>57.7</v>
+        <v>30</v>
       </c>
       <c r="D5" cm="1">
         <f t="array" ref="D5:F5">D3:F3</f>
@@ -2899,7 +3318,7 @@
       </c>
       <c r="G5">
         <f>VLT_jeHaus_FBH!E56</f>
-        <v>41.499387888201113</v>
+        <v>11.316499227839616</v>
       </c>
       <c r="H5">
         <f t="shared" ref="H5:H6" si="0">H4</f>
@@ -2912,11 +3331,11 @@
       </c>
       <c r="B6">
         <f>VLT_jeHaus_FBH!F53</f>
-        <v>70.900000000000006</v>
+        <v>35</v>
       </c>
       <c r="C6">
         <f>VLT_jeHaus_FBH!F54</f>
-        <v>60.9</v>
+        <v>30</v>
       </c>
       <c r="D6" cm="1">
         <f t="array" ref="D6:F6">D3:F3</f>
@@ -2930,7 +3349,7 @@
       </c>
       <c r="G6">
         <f>VLT_jeHaus_FBH!F56</f>
-        <v>44.713784610927043</v>
+        <v>11.316499227839616</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>

</xml_diff>